<commit_message>
clean up large accuracy check update
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_spikein_hbrown_09.06.19.xlsx
+++ b/fastqFiles/fastq_spikein_hbrown_09.06.19.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="16">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">fastqFileName</t>
   </si>
   <si>
-    <t xml:space="preserve">09.6.19</t>
+    <t xml:space="preserve">09.06.19</t>
   </si>
   <si>
     <t xml:space="preserve">H.BROWN</t>
@@ -67,16 +67,7 @@
     <t xml:space="preserve">spikein </t>
   </si>
   <si>
-    <t xml:space="preserve">09.6.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09.6.21</t>
-  </si>
-  <si>
     <t xml:space="preserve">na</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09.6.22</t>
   </si>
 </sst>
 </file>
@@ -233,7 +224,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,7 +486,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -521,7 +512,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
@@ -547,7 +538,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
@@ -573,7 +564,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>13</v>
@@ -599,7 +590,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -625,7 +616,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>13</v>
@@ -651,7 +642,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>13</v>
@@ -677,7 +668,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
@@ -703,7 +694,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>13</v>
@@ -729,7 +720,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>13</v>
@@ -755,7 +746,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
@@ -781,7 +772,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>13</v>
@@ -807,7 +798,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
@@ -822,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>2</v>
@@ -833,7 +824,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>13</v>
@@ -848,12 +839,12 @@
         <v>14</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
@@ -868,12 +859,12 @@
         <v>14</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>13</v>
@@ -888,12 +879,12 @@
         <v>14</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
@@ -908,12 +899,12 @@
         <v>14</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>13</v>
@@ -928,12 +919,12 @@
         <v>14</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>13</v>
@@ -948,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>